<commit_message>
save before move around
</commit_message>
<xml_diff>
--- a/excelhere/room_two.xlsx
+++ b/excelhere/room_two.xlsx
@@ -444,17 +444,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>234</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel </t>
+          <t>234</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>234</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">

</xml_diff>